<commit_message>
configuração de ambiente de treinamento
</commit_message>
<xml_diff>
--- a/dataSet.xlsx
+++ b/dataSet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno.brito\Downloads\ferramentas de modelagem\Modelo 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c67fd77eff8119b6/Educação/Projetos e Estudos autonomos/QuiosqueML/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_A4E6EBFE12D611BB5AABB057CB49C2B3C69084A6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22195544-2C41-D44D-84BC-01B7C0D91F62}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
+    <workbookView xWindow="-2100" yWindow="-21100" windowWidth="33600" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dados" sheetId="1" r:id="rId1"/>
@@ -47,13 +48,7 @@
     <t>Volume concreto (m3)</t>
   </si>
   <si>
-    <t>Area forma (m²)</t>
-  </si>
-  <si>
     <t>Peso de aço (kg)</t>
-  </si>
-  <si>
-    <t>Volume madeira (m³)</t>
   </si>
   <si>
     <t>Raio (m)</t>
@@ -73,11 +68,17 @@
   <si>
     <t>Carregamento pilar (Kn/m2)</t>
   </si>
+  <si>
+    <t>Area forma (m2)</t>
+  </si>
+  <si>
+    <t>Volume madeira (m2)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -423,59 +424,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
     <col min="3" max="3" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="1"/>
+    <col min="9" max="9" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" s="3" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" s="3" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>4</v>
@@ -490,19 +491,19 @@
         <v>6</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="P1" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
         <v>3</v>
       </c>
@@ -552,7 +553,7 @@
         <v>24264.783261505199</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>3.5</v>
       </c>
@@ -602,7 +603,7 @@
         <v>33904.030707254497</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>4</v>
       </c>
@@ -652,7 +653,7 @@
         <v>46308.213439018196</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>4.5</v>
       </c>
@@ -702,7 +703,7 @@
         <v>61864.674777500302</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>5</v>
       </c>
@@ -752,7 +753,7 @@
         <v>61864.674777500302</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>5.5</v>
       </c>
@@ -802,7 +803,7 @@
         <v>103983.80655743599</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -852,7 +853,7 @@
         <v>131338.186238011</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>3</v>
       </c>
@@ -902,7 +903,7 @@
         <v>28669.326887898402</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>3.5</v>
       </c>
@@ -952,7 +953,7 @@
         <v>37783.581901611396</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>4</v>
       </c>
@@ -1002,7 +1003,7 @@
         <v>49135.436690921</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>4.5</v>
       </c>
@@ -1052,7 +1053,7 @@
         <v>63032.708647159998</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>5</v>
       </c>
@@ -1102,7 +1103,7 @@
         <v>79783.215161661195</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>5.5</v>
       </c>
@@ -1152,7 +1153,7 @@
         <v>99694.773625757603</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>6</v>
       </c>
@@ -1202,7 +1203,7 @@
         <v>123075.20143078201</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>3</v>
       </c>
@@ -1252,7 +1253,7 @@
         <v>25874.6431078147</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>3.5</v>
       </c>
@@ -1302,7 +1303,7 @@
         <v>33316.6311654811</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>4</v>
       </c>
@@ -1352,7 +1353,7 @@
         <v>42528.247109320298</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>4.5</v>
       </c>
@@ -1402,7 +1403,7 @@
         <v>53748.190433210897</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>5</v>
       </c>
@@ -1452,7 +1453,7 @@
         <v>67215.160631031293</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>5.5</v>
       </c>
@@ -1502,7 +1503,7 @@
         <v>83167.857196659999</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>6</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>101844.979623976</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>3</v>
       </c>
@@ -1602,7 +1603,7 @@
         <v>23490.554904342102</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
         <v>3.5</v>
       </c>
@@ -1652,7 +1653,7 @@
         <v>29659.784532253601</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
         <v>4</v>
       </c>
@@ -1702,7 +1703,7 @@
         <v>37254.617509067401</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
         <v>4.5</v>
       </c>
@@ -1752,7 +1753,7 @@
         <v>46463.281916373599</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
         <v>5</v>
       </c>
@@ -1802,7 +1803,7 @@
         <v>57474.005835762102</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" s="1">
         <v>5.5</v>
       </c>
@@ -1852,7 +1853,7 @@
         <v>70475.017348823298</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
         <v>6</v>
       </c>
@@ -1902,7 +1903,7 @@
         <v>85654.544537146998</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
         <v>3</v>
       </c>
@@ -1952,7 +1953,7 @@
         <v>21777.3267261578</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B31" s="1">
         <v>3.5</v>
       </c>
@@ -2002,7 +2003,7 @@
         <v>27044.622801642901</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B32" s="1">
         <v>4</v>
       </c>
@@ -2052,7 +2053,7 @@
         <v>33500.615962631098</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B33" s="1">
         <v>4.5</v>
       </c>
@@ -2102,7 +2103,7 @@
         <v>41298.857231558497</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" s="1">
         <v>5</v>
       </c>
@@ -2152,7 +2153,7 @@
         <v>50592.897630861196</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" s="1">
         <v>5.5</v>
       </c>
@@ -2202,7 +2203,7 @@
         <v>61719.994674929803</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B36" s="1">
         <v>6</v>
       </c>
@@ -2252,7 +2253,7 @@
         <v>74521.080900642904</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B37" s="1">
         <v>3</v>
       </c>
@@ -2302,7 +2303,7 @@
         <v>20517.253412990998</v>
       </c>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B38" s="1">
         <v>3.5</v>
       </c>
@@ -2352,7 +2353,7 @@
         <v>25102.190000448099</v>
       </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B39" s="1">
         <v>4</v>
       </c>
@@ -2402,7 +2403,7 @@
         <v>30698.613003741299</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B40" s="1">
         <v>4.5</v>
       </c>
@@ -2452,7 +2453,7 @@
         <v>37434.202213801997</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B41" s="1">
         <v>5</v>
       </c>
@@ -2502,7 +2503,7 @@
         <v>45436.6374215619</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B42" s="1">
         <v>5.5</v>
       </c>
@@ -2552,7 +2553,7 @@
         <v>54833.598417952599</v>
       </c>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B43" s="1">
         <v>6</v>
       </c>
@@ -2602,7 +2603,7 @@
         <v>65752.764993905701</v>
       </c>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B44" s="1">
         <v>3</v>
       </c>
@@ -2652,7 +2653,7 @@
         <v>19622.707714910499</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" s="1">
         <v>3.5</v>
       </c>
@@ -2702,7 +2703,7 @@
         <v>23698.535939228001</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B46" s="1">
         <v>4</v>
       </c>
@@ -2752,7 +2753,7 @@
         <v>28656.1815014936</v>
       </c>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B47" s="1">
         <v>4.5</v>
       </c>
@@ -2802,7 +2803,7 @@
         <v>34604.412264324397</v>
       </c>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B48" s="1">
         <v>5</v>
       </c>
@@ -2852,7 +2853,7 @@
         <v>41651.996090337598</v>
       </c>
     </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B49" s="1">
         <v>5.5</v>
       </c>
@@ -2902,7 +2903,7 @@
         <v>49907.700842150502</v>
       </c>
     </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B50" s="1">
         <v>6</v>
       </c>
@@ -2952,7 +2953,7 @@
         <v>59480.294382380198</v>
       </c>
     </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B51" s="1">
         <v>3</v>
       </c>
@@ -3002,7 +3003,7 @@
         <v>18974.301496962002</v>
       </c>
     </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B52" s="1">
         <v>3.5</v>
       </c>
@@ -3052,7 +3053,7 @@
         <v>22653.110280450099</v>
       </c>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B53" s="1">
         <v>4</v>
       </c>
@@ -3102,7 +3103,7 @@
         <v>27113.850234719001</v>
       </c>
     </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B54" s="1">
         <v>4.5</v>
       </c>
@@ -3152,7 +3153,7 @@
         <v>32450.738718709501</v>
       </c>
     </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B55" s="1">
         <v>5</v>
       </c>
@@ -3202,7 +3203,7 @@
         <v>38757.993091362601</v>
       </c>
     </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B56" s="1">
         <v>5.5</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>46129.830711619201</v>
       </c>
     </row>
-    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B57" s="1">
         <v>6</v>
       </c>
@@ -3302,7 +3303,7 @@
         <v>54660.468938420003</v>
       </c>
     </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B58" s="1">
         <v>3.5</v>
       </c>
@@ -3352,7 +3353,7 @@
         <v>21870.534936248401</v>
       </c>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B59" s="1">
         <v>3</v>
       </c>
@@ -3402,7 +3403,7 @@
         <v>18500.774078299299</v>
       </c>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B60" s="1">
         <v>4</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>25937.680450682201</v>
       </c>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B61" s="1">
         <v>4.5</v>
       </c>
@@ -3502,7 +3503,7 @@
         <v>30791.227892157502</v>
       </c>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B62" s="1">
         <v>5</v>
       </c>
@@ -3552,7 +3553,7 @@
         <v>36513.992507295901</v>
       </c>
     </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B63" s="1">
         <v>5.5</v>
       </c>
@@ -3602,7 +3603,7 @@
         <v>43188.789542718798</v>
       </c>
     </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B64" s="1">
         <v>6</v>
       </c>
@@ -3652,7 +3653,7 @@
         <v>50898.4342450478</v>
       </c>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B65" s="1">
         <v>3</v>
       </c>
@@ -3702,7 +3703,7 @@
         <v>18172.482901456799</v>
       </c>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B66" s="1">
         <v>3.5</v>
       </c>
@@ -3752,7 +3753,7 @@
         <v>21280.3512269239</v>
       </c>
     </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B67" s="1">
         <v>4</v>
       </c>
@@ -3802,7 +3803,7 @@
         <v>25028.938711484101</v>
       </c>
     </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B68" s="1">
         <v>4.5</v>
       </c>
@@ -3852,7 +3853,7 @@
         <v>29491.918498511401</v>
       </c>
     </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B69" s="1">
         <v>5</v>
       </c>
@@ -3902,7 +3903,7 @@
         <v>34742.963731379801</v>
       </c>
     </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B70" s="1">
         <v>5.5</v>
       </c>
@@ -3952,7 +3953,7 @@
         <v>40855.7475534634</v>
       </c>
     </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B71" s="1">
         <v>6</v>
       </c>
@@ -4002,7 +4003,7 @@
         <v>47903.943108135798</v>
       </c>
     </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B72" s="1">
         <v>3</v>
       </c>
@@ -4052,7 +4053,7 @@
         <v>20266.596360845899</v>
       </c>
     </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B73" s="1">
         <v>3.5</v>
       </c>
@@ -4102,7 +4103,7 @@
         <v>30833.931162076198</v>
       </c>
     </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B74" s="1">
         <v>4</v>
       </c>
@@ -4152,7 +4153,7 @@
         <v>44702.304566150997</v>
       </c>
     </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B75" s="1">
         <v>4.5</v>
       </c>
@@ -4202,7 +4203,7 @@
         <v>62330.847326877403</v>
       </c>
     </row>
-    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B76" s="1">
         <v>5</v>
       </c>
@@ -4252,7 +4253,7 @@
         <v>84178.690198062701</v>
       </c>
     </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B77" s="1">
         <v>5.5</v>
       </c>
@@ -4302,7 +4303,7 @@
         <v>110704.96393351399</v>
       </c>
     </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B78" s="1">
         <v>6</v>
       </c>
@@ -4352,7 +4353,7 @@
         <v>142385.821884751</v>
       </c>
     </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B79" s="1">
         <v>3</v>
       </c>
@@ -4402,7 +4403,7 @@
         <v>22336.680327665799</v>
       </c>
     </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B80" s="1">
         <v>3.5</v>
       </c>
@@ -4452,7 +4453,7 @@
         <v>26669.840104145602</v>
       </c>
     </row>
-    <row r="81" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B81" s="1">
         <v>4</v>
       </c>
@@ -4502,7 +4503,7 @@
         <v>38175.829234974401</v>
       </c>
     </row>
-    <row r="82" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B82" s="1">
         <v>4.5</v>
       </c>
@@ -4552,7 +4553,7 @@
         <v>52646.345475506401</v>
       </c>
     </row>
-    <row r="83" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B83" s="1">
         <v>5</v>
       </c>
@@ -4602,7 +4603,7 @@
         <v>70478.951630627504</v>
       </c>
     </row>
-    <row r="84" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B84" s="1">
         <v>5.5</v>
       </c>
@@ -4652,7 +4653,7 @@
         <v>92032.080764714396</v>
       </c>
     </row>
-    <row r="85" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B85" s="1">
         <v>6</v>
       </c>
@@ -4702,7 +4703,7 @@
         <v>117664.165942144</v>
       </c>
     </row>
-    <row r="86" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B86" s="1">
         <v>3</v>
       </c>
@@ -4752,7 +4753,7 @@
         <v>19095.977674975202</v>
       </c>
     </row>
-    <row r="87" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B87" s="1">
         <v>3.5</v>
       </c>
@@ -4802,7 +4803,7 @@
         <v>26834.3441746627</v>
       </c>
     </row>
-    <row r="88" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B88" s="1">
         <v>4</v>
       </c>
@@ -4852,7 +4853,7 @@
         <v>36628.519204653297</v>
       </c>
     </row>
-    <row r="89" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B89" s="1">
         <v>4.5</v>
       </c>
@@ -4902,7 +4903,7 @@
         <v>48773.841288033298</v>
       </c>
     </row>
-    <row r="90" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B90" s="1">
         <v>5</v>
       </c>
@@ -4952,7 +4953,7 @@
         <v>63544.026920448501</v>
       </c>
     </row>
-    <row r="91" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B91" s="1">
         <v>5.5</v>
       </c>
@@ -5002,7 +5003,7 @@
         <v>81212.792597544496</v>
       </c>
     </row>
-    <row r="92" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B92" s="1">
         <v>6</v>
       </c>
@@ -5052,7 +5053,7 @@
         <v>102053.854814968</v>
       </c>
     </row>
-    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B93" s="1">
         <v>3</v>
       </c>
@@ -5102,7 +5103,7 @@
         <v>16607.229055539901</v>
       </c>
     </row>
-    <row r="94" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B94" s="1">
         <v>3.5</v>
       </c>
@@ -5152,7 +5153,7 @@
         <v>23038.7178011172</v>
       </c>
     </row>
-    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B95" s="1">
         <v>4</v>
       </c>
@@ -5202,7 +5203,7 @@
         <v>31125.917644916699</v>
       </c>
     </row>
-    <row r="96" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B96" s="1">
         <v>4.5</v>
       </c>
@@ -5252,7 +5253,7 @@
         <v>41100.3633455776</v>
       </c>
     </row>
-    <row r="97" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B97" s="1">
         <v>5</v>
       </c>
@@ -5302,7 +5303,7 @@
         <v>53175.939395415102</v>
       </c>
     </row>
-    <row r="98" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B98" s="1">
         <v>5.5</v>
       </c>
@@ -5352,7 +5353,7 @@
         <v>67566.530286744106</v>
       </c>
     </row>
-    <row r="99" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B99" s="1">
         <v>6</v>
       </c>
@@ -5402,7 +5403,7 @@
         <v>84486.020511879804</v>
       </c>
     </row>
-    <row r="100" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B100" s="1">
         <v>3</v>
       </c>
@@ -5452,7 +5453,7 @@
         <v>14808.271360566599</v>
       </c>
     </row>
-    <row r="101" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B101" s="1">
         <v>3.5</v>
       </c>
@@ -5502,7 +5503,7 @@
         <v>20313.017775512199</v>
       </c>
     </row>
-    <row r="102" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B102" s="1">
         <v>4</v>
       </c>
@@ -5552,7 +5553,7 @@
         <v>27194.107750319901</v>
       </c>
     </row>
-    <row r="103" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B103" s="1">
         <v>4.5</v>
       </c>
@@ -5602,7 +5603,7 @@
         <v>35638.6432770182</v>
       </c>
     </row>
-    <row r="104" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B104" s="1">
         <v>5</v>
       </c>
@@ -5652,7 +5653,7 @@
         <v>45818.875819916902</v>
       </c>
     </row>
-    <row r="105" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B105" s="1">
         <v>5.5</v>
       </c>
@@ -5702,7 +5703,7 @@
         <v>57907.0568433261</v>
       </c>
     </row>
-    <row r="106" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B106" s="1">
         <v>6</v>
       </c>
@@ -5752,7 +5753,7 @@
         <v>72075.437811555603</v>
       </c>
     </row>
-    <row r="107" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B107" s="1">
         <v>3</v>
       </c>
@@ -5802,7 +5803,7 @@
         <v>13487.243444899101</v>
       </c>
     </row>
-    <row r="108" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B108" s="1">
         <v>3.5</v>
       </c>
@@ -5852,7 +5853,7 @@
         <v>18316.208284014301</v>
       </c>
     </row>
-    <row r="109" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B109" s="1">
         <v>4</v>
       </c>
@@ -5902,7 +5903,7 @@
         <v>24319.760792766199</v>
       </c>
     </row>
-    <row r="110" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B110" s="1">
         <v>4.5</v>
       </c>
@@ -5952,7 +5953,7 @@
         <v>31653.280772001501</v>
       </c>
     </row>
-    <row r="111" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B111" s="1">
         <v>5</v>
       </c>
@@ -6002,7 +6003,7 @@
         <v>40459.064925965402</v>
       </c>
     </row>
-    <row r="112" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B112" s="1">
         <v>5.5</v>
       </c>
@@ -6052,7 +6053,7 @@
         <v>50879.409958903103</v>
       </c>
     </row>
-    <row r="113" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B113" s="1">
         <v>6</v>
       </c>
@@ -6102,7 +6103,7 @@
         <v>63056.612575059597</v>
       </c>
     </row>
-    <row r="114" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B114" s="1">
         <v>3</v>
       </c>
@@ -6152,7 +6153,7 @@
         <v>12505.610075790901</v>
       </c>
     </row>
-    <row r="115" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B115" s="1">
         <v>3.5</v>
       </c>
@@ -6202,7 +6203,7 @@
         <v>16831.204157288001</v>
       </c>
     </row>
-    <row r="116" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B116" s="1">
         <v>4</v>
       </c>
@@ -6252,7 +6253,7 @@
         <v>22184.230112127301</v>
       </c>
     </row>
-    <row r="117" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B117" s="1">
         <v>4.5</v>
       </c>
@@ -6302,7 +6303,7 @@
         <v>28695.628819288399</v>
       </c>
     </row>
-    <row r="118" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B118" s="1">
         <v>5</v>
       </c>
@@ -6352,7 +6353,7 @@
         <v>36485.718177616603</v>
       </c>
     </row>
-    <row r="119" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B119" s="1">
         <v>5.5</v>
       </c>
@@ -6402,7 +6403,7 @@
         <v>45674.816085957398</v>
       </c>
     </row>
-    <row r="120" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B120" s="1">
         <v>6</v>
       </c>
@@ -6452,7 +6453,7 @@
         <v>56383.240443155999</v>
       </c>
     </row>
-    <row r="121" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B121" s="1">
         <v>3</v>
       </c>
@@ -6502,7 +6503,7 @@
         <v>11751.844365905899</v>
       </c>
     </row>
-    <row r="122" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B122" s="1">
         <v>3.5</v>
       </c>
@@ -6552,7 +6553,7 @@
         <v>15688.933865197199</v>
       </c>
     </row>
-    <row r="123" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B123" s="1">
         <v>4</v>
       </c>
@@ -6602,7 +6603,7 @@
         <v>20540.2919466641</v>
       </c>
     </row>
-    <row r="124" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B124" s="1">
         <v>4.5</v>
       </c>
@@ -6652,7 +6653,7 @@
         <v>26418.4951513339</v>
       </c>
     </row>
-    <row r="125" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B125" s="1">
         <v>5</v>
       </c>
@@ -6702,7 +6703,7 @@
         <v>33427.033101082103</v>
       </c>
     </row>
-    <row r="126" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B126" s="1">
         <v>5.5</v>
       </c>
@@ -6752,7 +6753,7 @@
         <v>41669.395417784603</v>
       </c>
     </row>
-    <row r="127" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B127" s="1">
         <v>6</v>
       </c>
@@ -6802,7 +6803,7 @@
         <v>51249.071723316803</v>
       </c>
     </row>
-    <row r="128" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B128" s="1">
         <v>3</v>
       </c>
@@ -6852,7 +6853,7 @@
         <v>11416.320975705499</v>
       </c>
     </row>
-    <row r="129" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B129" s="1">
         <v>3.5</v>
       </c>
@@ -6902,7 +6903,7 @@
         <v>15310.524416149899</v>
       </c>
     </row>
-    <row r="130" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B130" s="1">
         <v>4</v>
       </c>
@@ -6952,7 +6953,7 @@
         <v>20118.9964387699</v>
       </c>
     </row>
-    <row r="131" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B131" s="1">
         <v>4.5</v>
       </c>
@@ -7002,7 +7003,7 @@
         <v>25954.313584592801</v>
       </c>
     </row>
-    <row r="132" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B132" s="1">
         <v>5</v>
       </c>
@@ -7052,7 +7053,7 @@
         <v>32919.965475494202</v>
       </c>
     </row>
-    <row r="133" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B133" s="1">
         <v>5.5</v>
       </c>
@@ -7102,7 +7103,7 @@
         <v>41119.441733349697</v>
       </c>
     </row>
-    <row r="134" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B134" s="1">
         <v>6</v>
       </c>
@@ -7152,7 +7153,7 @@
         <v>50656.231980035001</v>
       </c>
     </row>
-    <row r="135" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B135" s="1">
         <v>3</v>
       </c>
@@ -7202,7 +7203,7 @@
         <v>11165.9186773562</v>
       </c>
     </row>
-    <row r="136" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B136" s="1">
         <v>3.5</v>
       </c>
@@ -7252,7 +7253,7 @@
         <v>14798.263849952</v>
       </c>
     </row>
-    <row r="137" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B137" s="1">
         <v>4</v>
       </c>
@@ -7302,7 +7303,7 @@
         <v>19256.8345796791</v>
       </c>
     </row>
-    <row r="138" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B138" s="1">
         <v>4.5</v>
       </c>
@@ -7352,7 +7353,7 @@
         <v>24639.962441218198</v>
       </c>
     </row>
-    <row r="139" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B139" s="1">
         <v>5</v>
       </c>
@@ -7402,7 +7403,7 @@
         <v>31038.0657371366</v>
       </c>
     </row>
-    <row r="140" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B140" s="1">
         <v>5.5</v>
       </c>
@@ -7452,7 +7453,7 @@
         <v>38541.562770001903</v>
       </c>
     </row>
-    <row r="141" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B141" s="1">
         <v>6</v>
       </c>
@@ -7502,7 +7503,7 @@
         <v>47240.871842381501</v>
       </c>
     </row>
-    <row r="142" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B142" s="1">
         <v>3</v>
       </c>
@@ -7552,7 +7553,7 @@
         <v>10702.269944981201</v>
       </c>
     </row>
-    <row r="143" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B143" s="1">
         <v>3.5</v>
       </c>
@@ -7602,7 +7603,7 @@
         <v>14089.6858559636</v>
       </c>
     </row>
-    <row r="144" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B144" s="1">
         <v>4</v>
       </c>
@@ -7652,7 +7653,7 @@
         <v>18233.414733867401</v>
       </c>
     </row>
-    <row r="145" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B145" s="1">
         <v>4.5</v>
       </c>
@@ -7702,7 +7703,7 @@
         <v>23220.177189162801</v>
       </c>
     </row>
-    <row r="146" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B146" s="1">
         <v>5</v>
       </c>
@@ -7752,7 +7753,7 @@
         <v>29129.9829525071</v>
       </c>
     </row>
-    <row r="147" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B147" s="1">
         <v>5.5</v>
       </c>
@@ -7802,7 +7803,7 @@
         <v>36042.841754558198</v>
       </c>
     </row>
-    <row r="148" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B148" s="1">
         <v>6</v>
       </c>
@@ -7852,7 +7853,7 @@
         <v>44038.763325973101</v>
       </c>
     </row>
-    <row r="149" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B149" s="1">
         <v>3</v>
       </c>
@@ -7902,7 +7903,7 @@
         <v>21084.9342146116</v>
       </c>
     </row>
-    <row r="150" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B150" s="1">
         <v>3.5</v>
       </c>
@@ -7952,7 +7953,7 @@
         <v>29631.381443268001</v>
       </c>
     </row>
-    <row r="151" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B151" s="1">
         <v>4</v>
       </c>
@@ -8002,7 +8003,7 @@
         <v>40668.302021389398</v>
       </c>
     </row>
-    <row r="152" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B152" s="1">
         <v>4.5</v>
       </c>
@@ -8052,7 +8053,7 @@
         <v>54543.8304216014</v>
       </c>
     </row>
-    <row r="153" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B153" s="1">
         <v>5</v>
       </c>
@@ -8102,7 +8103,7 @@
         <v>71606.101116529695</v>
       </c>
     </row>
-    <row r="154" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B154" s="1">
         <v>5.5</v>
       </c>
@@ -8152,7 +8153,7 @@
         <v>92203.248578799801</v>
       </c>
     </row>
-    <row r="155" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B155" s="1">
         <v>6</v>
       </c>
@@ -8202,7 +8203,7 @@
         <v>116700.42987875101</v>
       </c>
     </row>
-    <row r="156" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B156" s="1">
         <v>3</v>
       </c>
@@ -8252,7 +8253,7 @@
         <v>31940.129241468399</v>
       </c>
     </row>
-    <row r="157" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B157" s="1">
         <v>3.5</v>
       </c>
@@ -8302,7 +8303,7 @@
         <v>41026.882019109798</v>
       </c>
     </row>
-    <row r="158" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B158" s="1">
         <v>4</v>
       </c>
@@ -8352,7 +8353,7 @@
         <v>52086.9410515786</v>
       </c>
     </row>
-    <row r="159" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B159" s="1">
         <v>4.5</v>
       </c>
@@ -8402,7 +8403,7 @@
         <v>65390.367512954901</v>
       </c>
     </row>
-    <row r="160" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B160" s="1">
         <v>5</v>
       </c>
@@ -8452,7 +8453,7 @@
         <v>81207.222577318695</v>
       </c>
     </row>
-    <row r="161" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B161" s="1">
         <v>5.5</v>
       </c>
@@ -8502,7 +8503,7 @@
         <v>99807.567418750303</v>
       </c>
     </row>
-    <row r="162" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B162" s="1">
         <v>6</v>
       </c>
@@ -8552,7 +8553,7 @@
         <v>121461.46321133</v>
       </c>
     </row>
-    <row r="163" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B163" s="1">
         <v>3</v>
       </c>
@@ -8602,7 +8603,7 @@
         <v>29368.795749451601</v>
       </c>
     </row>
-    <row r="164" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B164" s="1">
         <v>3.5</v>
       </c>
@@ -8652,7 +8653,7 @@
         <v>36874.380214172503</v>
       </c>
     </row>
-    <row r="165" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B165" s="1">
         <v>4</v>
       </c>
@@ -8702,7 +8703,7 @@
         <v>45910.163780504001</v>
       </c>
     </row>
-    <row r="166" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B166" s="1">
         <v>4.5</v>
       </c>
@@ -8752,7 +8753,7 @@
         <v>56680.641830244298</v>
       </c>
     </row>
-    <row r="167" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B167" s="1">
         <v>5</v>
       </c>
@@ -8802,7 +8803,7 @@
         <v>69390.309745191407</v>
       </c>
     </row>
-    <row r="168" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B168" s="1">
         <v>5.5</v>
       </c>
@@ -8852,7 +8853,7 @@
         <v>84243.662907143706</v>
       </c>
     </row>
-    <row r="169" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B169" s="1">
         <v>6</v>
       </c>
@@ -8902,7 +8903,7 @@
         <v>101445.19669789899</v>
       </c>
     </row>
-    <row r="170" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B170" s="1">
         <v>3</v>
       </c>
@@ -8952,7 +8953,7 @@
         <v>27137.964904685199</v>
       </c>
     </row>
-    <row r="171" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B171" s="1">
         <v>3.5</v>
       </c>
@@ -9002,7 +9003,7 @@
         <v>33465.868421492203</v>
       </c>
     </row>
-    <row r="172" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B172" s="1">
         <v>4</v>
       </c>
@@ -9052,7 +9053,7 @@
         <v>41012.039389742204</v>
       </c>
     </row>
-    <row r="173" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B173" s="1">
         <v>4.5</v>
       </c>
@@ -9102,7 +9103,7 @@
         <v>49935.086477102501</v>
       </c>
     </row>
-    <row r="174" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B174" s="1">
         <v>5</v>
       </c>
@@ -9152,7 +9153,7 @@
         <v>60393.618351240599</v>
       </c>
     </row>
-    <row r="175" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B175" s="1">
         <v>5.5</v>
       </c>
@@ -9202,7 +9203,7 @@
         <v>72546.243679823703</v>
       </c>
     </row>
-    <row r="176" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B176" s="1">
         <v>6</v>
       </c>
@@ -9252,7 +9253,7 @@
         <v>86551.571130519194</v>
       </c>
     </row>
-    <row r="177" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B177" s="1">
         <v>3</v>
       </c>
@@ -9302,7 +9303,7 @@
         <v>25511.254878997301</v>
       </c>
     </row>
-    <row r="178" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B178" s="1">
         <v>3.5</v>
       </c>
@@ -9352,7 +9353,7 @@
         <v>31003.135390715499</v>
       </c>
     </row>
-    <row r="179" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B179" s="1">
         <v>4</v>
       </c>
@@ -9402,7 +9403,7 @@
         <v>37500.1421005952</v>
       </c>
     </row>
-    <row r="180" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B180" s="1">
         <v>4.5</v>
       </c>
@@ -9452,7 +9453,7 @@
         <v>45129.601618595101</v>
       </c>
     </row>
-    <row r="181" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B181" s="1">
         <v>5</v>
       </c>
@@ -9502,7 +9503,7 @@
         <v>54018.840554674003</v>
       </c>
     </row>
-    <row r="182" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B182" s="1">
         <v>5.5</v>
       </c>
@@ -9552,7 +9553,7 @@
         <v>64295.185518790502</v>
       </c>
     </row>
-    <row r="183" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B183" s="1">
         <v>6</v>
       </c>
@@ -9602,7 +9603,7 @@
         <v>76085.963120903398</v>
       </c>
     </row>
-    <row r="184" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B184" s="1">
         <v>3</v>
       </c>
@@ -9652,7 +9653,7 @@
         <v>24312.381048216201</v>
       </c>
     </row>
-    <row r="185" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B185" s="1">
         <v>3.5</v>
       </c>
@@ -9702,7 +9703,7 @@
         <v>29174.175443011402</v>
       </c>
     </row>
-    <row r="186" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B186" s="1">
         <v>4</v>
       </c>
@@ -9752,7 +9753,7 @@
         <v>34883.303885089001</v>
       </c>
     </row>
-    <row r="187" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B187" s="1">
         <v>4.5</v>
       </c>
@@ -9802,7 +9803,7 @@
         <v>41543.9958270157</v>
       </c>
     </row>
-    <row r="188" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B188" s="1">
         <v>5</v>
       </c>
@@ -9852,7 +9853,7 @@
         <v>49260.480721358399</v>
       </c>
     </row>
-    <row r="189" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B189" s="1">
         <v>5.5</v>
       </c>
@@ -9902,7 +9903,7 @@
         <v>58136.988020683799</v>
       </c>
     </row>
-    <row r="190" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B190" s="1">
         <v>6</v>
       </c>
@@ -9952,7 +9953,7 @@
         <v>68277.747177558704</v>
       </c>
     </row>
-    <row r="191" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B191" s="1">
         <v>3</v>
       </c>
@@ -10002,7 +10003,7 @@
         <v>23466.888347436401</v>
       </c>
     </row>
-    <row r="192" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B192" s="1">
         <v>3.5</v>
       </c>
@@ -10052,7 +10053,7 @@
         <v>27863.573649108999</v>
       </c>
     </row>
-    <row r="193" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B193" s="1">
         <v>4</v>
       </c>
@@ -10102,7 +10103,7 @@
         <v>32994.457968083902</v>
       </c>
     </row>
-    <row r="194" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B194" s="1">
         <v>4.5</v>
       </c>
@@ -10152,7 +10153,7 @@
         <v>38947.220835457301</v>
       </c>
     </row>
-    <row r="195" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B195" s="1">
         <v>5</v>
       </c>
@@ -10202,7 +10203,7 @@
         <v>45809.541782325599</v>
       </c>
     </row>
-    <row r="196" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B196" s="1">
         <v>5.5</v>
       </c>
@@ -10252,7 +10253,7 @@
         <v>53669.100339785298</v>
       </c>
     </row>
-    <row r="197" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B197" s="1">
         <v>6</v>
       </c>
@@ -10302,7 +10303,7 @@
         <v>62613.576038932799</v>
       </c>
     </row>
-    <row r="198" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B198" s="1">
         <v>3</v>
       </c>
@@ -10352,7 +10353,7 @@
         <v>22854.9304036166</v>
       </c>
     </row>
-    <row r="199" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B199" s="1">
         <v>3.5</v>
       </c>
@@ -10402,7 +10403,7 @@
         <v>26889.512282309701</v>
       </c>
     </row>
-    <row r="200" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B200" s="1">
         <v>4</v>
       </c>
@@ -10452,7 +10453,7 @@
         <v>31571.718382904699</v>
       </c>
     </row>
-    <row r="201" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B201" s="1">
         <v>4.5</v>
       </c>
@@ -10502,7 +10503,7 @@
         <v>36976.5793573599</v>
       </c>
     </row>
-    <row r="202" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B202" s="1">
         <v>5</v>
       </c>
@@ -10552,7 +10553,7 @@
         <v>43179.125857633298</v>
       </c>
     </row>
-    <row r="203" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B203" s="1">
         <v>5.5</v>
       </c>
@@ -10602,7 +10603,7 @@
         <v>50254.388535683203</v>
       </c>
     </row>
-    <row r="204" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B204" s="1">
         <v>6</v>
       </c>
@@ -10652,7 +10653,7 @@
         <v>58277.398043467903</v>
       </c>
     </row>
-    <row r="205" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B205" s="1">
         <v>3</v>
       </c>
@@ -10702,7 +10703,7 @@
         <v>22417.678564115799</v>
       </c>
     </row>
-    <row r="206" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B206" s="1">
         <v>3.5</v>
       </c>
@@ -10752,7 +10753,7 @@
         <v>26166.5257542297</v>
       </c>
     </row>
-    <row r="207" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B207" s="1">
         <v>4</v>
       </c>
@@ -10802,7 +10803,7 @@
         <v>30495.961753588599</v>
       </c>
     </row>
-    <row r="208" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B208" s="1">
         <v>4.5</v>
       </c>
@@ -10852,7 +10853,7 @@
         <v>35471.230684360198</v>
       </c>
     </row>
-    <row r="209" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B209" s="1">
         <v>5</v>
       </c>
@@ -10902,7 +10903,7 @@
         <v>41157.576668712303</v>
       </c>
     </row>
-    <row r="210" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B210" s="1">
         <v>5.5</v>
       </c>
@@ -10952,7 +10953,7 @@
         <v>47620.243828813</v>
       </c>
     </row>
-    <row r="211" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B211" s="1">
         <v>6</v>
       </c>
@@ -11002,7 +11003,7 @@
         <v>54924.4762868299</v>
       </c>
     </row>
-    <row r="212" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B212" s="1">
         <v>3</v>
       </c>
@@ -11052,7 +11053,7 @@
         <v>22107.798659240401</v>
       </c>
     </row>
-    <row r="213" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B213" s="1">
         <v>3.5</v>
       </c>
@@ -11102,7 +11103,7 @@
         <v>25625.785858200601</v>
       </c>
     </row>
-    <row r="214" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B214" s="1">
         <v>4</v>
       </c>
@@ -11152,7 +11153,7 @@
         <v>29671.0612534211</v>
       </c>
     </row>
-    <row r="215" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B215" s="1">
         <v>4.5</v>
       </c>
@@ -11202,7 +11203,7 @@
         <v>34301.0935650143</v>
       </c>
     </row>
-    <row r="216" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B216" s="1">
         <v>5</v>
       </c>
@@ -11252,7 +11253,7 @@
         <v>39573.351513092202</v>
       </c>
     </row>
-    <row r="217" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B217" s="1">
         <v>5.5</v>
       </c>
@@ -11302,7 +11303,7 @@
         <v>45545.303817767199</v>
       </c>
     </row>
-    <row r="218" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B218" s="1">
         <v>6</v>
       </c>

</xml_diff>